<commit_message>
Auto commit at 2025-09-28 11:31:57.15
</commit_message>
<xml_diff>
--- a/data/yyxl.xlsx
+++ b/data/yyxl.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="10">
   <si>
     <t>日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -33,19 +33,6 @@
     <t>高岭站</t>
   </si>
   <si>
-    <t>平均每小时充电功率(kw)</t>
-  </si>
-  <si>
-    <t>终端日均充电电量(kwh)</t>
-  </si>
-  <si>
-    <t>终端日均充电收益(元)</t>
-  </si>
-  <si>
-    <t>单枪日均充电次数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>终端日均利用率</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -53,14 +40,31 @@
     <t>终端日均充电时长(分钟)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>终端日均充电电量(kwh)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>终端日均充电收益(元)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>平均每小时充电功率(kw)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单枪日均充电次数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="176" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="179" formatCode="0.00_ "/>
+    <numFmt numFmtId="177" formatCode="0.00_ "/>
+    <numFmt numFmtId="184" formatCode="0.00_);[Red]\(0.00\)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -98,15 +102,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="184" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -411,23 +417,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O53"/>
+  <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="H61" sqref="H61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="12.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="22.5" customWidth="1"/>
-    <col min="4" max="4" width="16.75" customWidth="1"/>
+    <col min="4" max="4" width="16.75" style="6" customWidth="1"/>
     <col min="5" max="5" width="22.5" customWidth="1"/>
     <col min="6" max="6" width="24.125" customWidth="1"/>
     <col min="7" max="7" width="24.375" customWidth="1"/>
     <col min="8" max="8" width="25.125" customWidth="1"/>
     <col min="9" max="9" width="11.5" customWidth="1"/>
     <col min="10" max="10" width="12.875" customWidth="1"/>
+    <col min="12" max="12" width="10.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.15">
@@ -438,22 +445,22 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
@@ -2179,6 +2186,58 @@
       <c r="N53" s="3"/>
       <c r="O53" s="3"/>
     </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A54" s="1">
+        <v>45927</v>
+      </c>
+      <c r="B54" t="s">
+        <v>2</v>
+      </c>
+      <c r="C54" s="7">
+        <v>131.43307086614172</v>
+      </c>
+      <c r="D54" s="6">
+        <v>9.1272965879265089E-2</v>
+      </c>
+      <c r="E54" s="7">
+        <v>76.294960629921249</v>
+      </c>
+      <c r="F54" s="7">
+        <v>25.86669291338583</v>
+      </c>
+      <c r="G54" s="7">
+        <v>34.83</v>
+      </c>
+      <c r="H54" s="7">
+        <v>3.2125984251968505</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A55" s="1">
+        <v>45927</v>
+      </c>
+      <c r="B55" t="s">
+        <v>3</v>
+      </c>
+      <c r="C55" s="7">
+        <v>161.44444444444446</v>
+      </c>
+      <c r="D55" s="6">
+        <v>0.11211419753086421</v>
+      </c>
+      <c r="E55" s="7">
+        <v>115.24166666666666</v>
+      </c>
+      <c r="F55" s="7">
+        <v>27.656388888888888</v>
+      </c>
+      <c r="G55" s="7">
+        <v>42.828974535443912</v>
+      </c>
+      <c r="H55" s="7">
+        <v>4.333333333333333</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>